<commit_message>
calculation from excel entities
</commit_message>
<xml_diff>
--- a/docs/Materialy.xlsx
+++ b/docs/Materialy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\OcelisConfigurator\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\OcelisConfigurator\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFFD488-5EAA-479F-8896-B2EA26F8D314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2CDF6A-A016-4FD3-9512-E3EB8B843524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8067D1D9-A08F-4E6F-8F36-E765066A912A}"/>
+    <workbookView xWindow="14370" yWindow="0" windowWidth="37335" windowHeight="20985" xr2:uid="{8067D1D9-A08F-4E6F-8F36-E765066A912A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,15 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="30">
   <si>
-    <t>sedlovy_15</t>
-  </si>
-  <si>
-    <t>sedlovy_35</t>
-  </si>
-  <si>
-    <t>sedlovy_45</t>
-  </si>
-  <si>
     <t>plochy 3x0,3</t>
   </si>
   <si>
@@ -126,6 +117,15 @@
   </si>
   <si>
     <t>DelkaMaxMetry</t>
+  </si>
+  <si>
+    <t>SedlovySklon15</t>
+  </si>
+  <si>
+    <t>SedlovySklon35</t>
+  </si>
+  <si>
+    <t>SedlovySklon45</t>
   </si>
 </sst>
 </file>
@@ -173,7 +173,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -189,7 +189,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -509,637 +509,637 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
         <v>3</v>
       </c>
-      <c r="D2">
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>11</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
       </c>
       <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3">
         <v>14.6</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
       </c>
       <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4">
         <v>18.2</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
       </c>
       <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5">
         <v>21.733333330000001</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-      <c r="F5">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
       </c>
       <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6">
         <v>25.333333329999999</v>
-      </c>
-      <c r="E6">
-        <v>6</v>
-      </c>
-      <c r="F6">
-        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
       </c>
       <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7">
         <v>28.93333333</v>
-      </c>
-      <c r="E7">
-        <v>7</v>
-      </c>
-      <c r="F7">
-        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
+        <v>20</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
       </c>
       <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8">
         <v>12.133333329999999</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
       </c>
       <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9">
         <v>16.06666667</v>
-      </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
       </c>
       <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10">
         <v>19.93333333</v>
-      </c>
-      <c r="E10">
-        <v>4</v>
-      </c>
-      <c r="F10">
-        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
       </c>
       <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11">
         <v>23.866666670000001</v>
-      </c>
-      <c r="E11">
-        <v>5</v>
-      </c>
-      <c r="F11">
-        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
       </c>
       <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12">
         <v>27.8</v>
-      </c>
-      <c r="E12">
-        <v>6</v>
-      </c>
-      <c r="F12">
-        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
       </c>
       <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13">
         <v>31.733333330000001</v>
-      </c>
-      <c r="E13">
-        <v>7</v>
-      </c>
-      <c r="F13">
-        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
       </c>
       <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14">
         <v>12.733333330000001</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
       </c>
       <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15">
         <v>17.666666670000001</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-      <c r="F15">
-        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
       </c>
       <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16">
         <v>22.466666669999999</v>
-      </c>
-      <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="F16">
-        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
       </c>
       <c r="D17">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17">
         <v>27.666666670000001</v>
-      </c>
-      <c r="E17">
-        <v>5</v>
-      </c>
-      <c r="F17">
-        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
       </c>
       <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18">
         <v>33.799999999999997</v>
-      </c>
-      <c r="E18">
-        <v>6</v>
-      </c>
-      <c r="F18">
-        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
       </c>
       <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19">
         <v>40.4</v>
-      </c>
-      <c r="E19">
-        <v>7</v>
-      </c>
-      <c r="F19">
-        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
       <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20">
         <v>15.866666670000001</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
       </c>
       <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21">
         <v>23.2</v>
-      </c>
-      <c r="E21">
-        <v>3</v>
-      </c>
-      <c r="F21">
-        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
       </c>
       <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22">
         <v>31</v>
-      </c>
-      <c r="E22">
-        <v>4</v>
-      </c>
-      <c r="F22">
-        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
       </c>
       <c r="D23">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23">
         <v>40</v>
-      </c>
-      <c r="E23">
-        <v>5</v>
-      </c>
-      <c r="F23">
-        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
       </c>
       <c r="D24">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24">
         <v>50.8</v>
-      </c>
-      <c r="E24">
-        <v>6</v>
-      </c>
-      <c r="F24">
-        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
       </c>
       <c r="D25">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25">
         <v>62.733333330000001</v>
-      </c>
-      <c r="E25">
-        <v>7</v>
-      </c>
-      <c r="F25">
-        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
         <v>2</v>
       </c>
-      <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26">
+      <c r="F26">
         <v>18.266666669999999</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
       </c>
       <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27">
         <v>27.333333329999999</v>
-      </c>
-      <c r="E27">
-        <v>3</v>
-      </c>
-      <c r="F27">
-        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
-      </c>
-      <c r="C28" t="s">
-        <v>11</v>
+        <v>19</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
       </c>
       <c r="D28">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28">
         <v>37.333333330000002</v>
-      </c>
-      <c r="E28">
-        <v>4</v>
-      </c>
-      <c r="F28">
-        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" t="s">
-        <v>14</v>
+        <v>19</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
       </c>
       <c r="D29">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29">
         <v>49.133333329999999</v>
-      </c>
-      <c r="E29">
-        <v>5</v>
-      </c>
-      <c r="F29">
-        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
       </c>
       <c r="D30">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30">
         <v>63.266666669999999</v>
-      </c>
-      <c r="E30">
-        <v>6</v>
-      </c>
-      <c r="F30">
-        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C31">
+        <v>7</v>
       </c>
       <c r="D31">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31">
         <v>78.933333329999996</v>
-      </c>
-      <c r="E31">
-        <v>7</v>
-      </c>
-      <c r="F31">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>